<commit_message>
Updated TLML 4 baseline
</commit_message>
<xml_diff>
--- a/data/SampleKeys.xlsx
+++ b/data/SampleKeys.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameronkerr/CapTCRRepo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cameronkerr/CapTCRRepo/CapTCR-TIL-Tracking/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB744C6-4889-3F49-A985-D1E965E72AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55F85A33-36FD-4640-8F68-750ABC156162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="880" windowWidth="27080" windowHeight="20220" xr2:uid="{C4CCCC86-406A-D64C-9D84-281E041E1E19}"/>
+    <workbookView xWindow="11440" yWindow="2680" windowWidth="27080" windowHeight="17540" xr2:uid="{C4CCCC86-406A-D64C-9D84-281E041E1E19}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -412,9 +412,6 @@
     <t>Initials</t>
   </si>
   <si>
-    <t>TLML_4_JR_baseline2_TCR-J_Dep_TCR-V_genomic_1000</t>
-  </si>
-  <si>
     <t>TLML_22_PJ_FU1_TCR-J_Dep_TCR-V_genomic_1000</t>
   </si>
   <si>
@@ -452,6 +449,9 @@
   </si>
   <si>
     <t>TLML-026-FT_A_B_DNA</t>
+  </si>
+  <si>
+    <t>17_02_TLML-004-JR-BL_TCR-J_D_TCR-V_genomic_1000</t>
   </si>
 </sst>
 </file>
@@ -833,8 +833,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D08BA8B-9E1F-1449-980B-C72CA36368AE}">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1297,17 +1297,17 @@
       <c r="C15" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="2" t="s">
         <v>24</v>
       </c>
       <c r="E15" s="4">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="F15" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G15" s="4">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>11</v>
@@ -1316,9 +1316,8 @@
         <v>12</v>
       </c>
       <c r="J15" t="s">
-        <v>125</v>
-      </c>
-      <c r="K15" s="1"/>
+        <v>138</v>
+      </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -3153,7 +3152,7 @@
         <v>12</v>
       </c>
       <c r="J71" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -3188,7 +3187,7 @@
         <v>12</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -3223,7 +3222,7 @@
         <v>12</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -3258,7 +3257,7 @@
         <v>12</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -3293,7 +3292,7 @@
         <v>12</v>
       </c>
       <c r="J75" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -3328,7 +3327,7 @@
         <v>12</v>
       </c>
       <c r="J76" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="K76" s="1"/>
     </row>
@@ -3361,7 +3360,7 @@
         <v>29</v>
       </c>
       <c r="J77" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K77" s="1"/>
     </row>
@@ -3394,7 +3393,7 @@
         <v>29</v>
       </c>
       <c r="J78" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="K78" s="1"/>
     </row>
@@ -3427,7 +3426,7 @@
         <v>29</v>
       </c>
       <c r="J79" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="K79" s="1"/>
     </row>
@@ -3460,7 +3459,7 @@
         <v>29</v>
       </c>
       <c r="J80" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K80" s="1"/>
     </row>
@@ -3493,7 +3492,7 @@
         <v>29</v>
       </c>
       <c r="J81" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="K81" s="1"/>
     </row>
@@ -3526,7 +3525,7 @@
         <v>29</v>
       </c>
       <c r="J82" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="K82" s="1"/>
     </row>
@@ -3559,7 +3558,7 @@
         <v>12</v>
       </c>
       <c r="J83" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="K83" s="1"/>
     </row>

</xml_diff>